<commit_message>
RTM UPDATE ( TC FOR BOOKING )
</commit_message>
<xml_diff>
--- a/Archive/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
+++ b/Archive/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="241">
   <si>
     <t>CR</t>
   </si>
@@ -699,6 +699,61 @@
 TAWA_Admin_012
 TAWA_Admin_013
 TAWA_Admin_017</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_01
+TAWA_BOOKING_17
+TAWA_BOOKING_13
+TAWA_BOOKING_14</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_01
+TAWA_BOOKING_10</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_01</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_02</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_03</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_04</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_05
+TAWA_BOOKING_12</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_18</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_06</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_07</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_08
+TAWA_BOOKING_09</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_01
+TAWA_BOOKING_03</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_011</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_15</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_052</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_16</t>
   </si>
 </sst>
 </file>
@@ -775,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -800,6 +855,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1105,26 +1169,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B105" workbookViewId="0">
-      <selection activeCell="H125" sqref="H125"/>
+    <sheetView tabSelected="1" topLeftCell="B99" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="24" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1213,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1166,7 +1230,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1186,7 +1250,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>112</v>
       </c>
@@ -1206,7 +1270,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>112</v>
       </c>
@@ -1226,7 +1290,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1246,7 +1310,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1266,7 +1330,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1286,7 +1350,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1306,7 +1370,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1326,7 +1390,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1346,7 +1410,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1366,7 +1430,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1386,7 +1450,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1406,7 +1470,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1426,7 +1490,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1510,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1466,7 +1530,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1486,7 +1550,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1506,7 +1570,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1529,7 +1593,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1546,7 +1610,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1563,7 +1627,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1583,7 +1647,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1603,7 +1667,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1623,7 +1687,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1643,7 +1707,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1660,7 +1724,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1677,7 +1741,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1694,7 +1758,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1714,7 +1778,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1734,7 +1798,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1754,7 +1818,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1774,7 +1838,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1794,7 +1858,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>114</v>
       </c>
@@ -1811,7 +1875,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>114</v>
       </c>
@@ -1828,7 +1892,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>114</v>
       </c>
@@ -1845,7 +1909,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>114</v>
       </c>
@@ -1862,7 +1926,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>114</v>
       </c>
@@ -1879,7 +1943,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>114</v>
       </c>
@@ -1896,7 +1960,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -1913,7 +1977,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -1930,7 +1994,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -1947,7 +2011,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -1964,7 +2028,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -1981,7 +2045,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -1998,7 +2062,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -2015,7 +2079,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -2035,7 +2099,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>112</v>
       </c>
@@ -2058,7 +2122,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>7</v>
       </c>
@@ -2081,7 +2145,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>7</v>
       </c>
@@ -2098,7 +2162,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>7</v>
       </c>
@@ -2115,7 +2179,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>165</v>
       </c>
@@ -2138,7 +2202,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>165</v>
       </c>
@@ -2161,7 +2225,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>165</v>
       </c>
@@ -2184,7 +2248,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>165</v>
       </c>
@@ -2207,7 +2271,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>165</v>
       </c>
@@ -2230,7 +2294,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>165</v>
       </c>
@@ -2254,7 +2318,7 @@
       </c>
       <c r="I58"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>117</v>
       </c>
@@ -2271,7 +2335,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>117</v>
       </c>
@@ -2288,7 +2352,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>117</v>
       </c>
@@ -2305,7 +2369,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>117</v>
       </c>
@@ -2322,7 +2386,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>114</v>
       </c>
@@ -2339,7 +2403,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>114</v>
       </c>
@@ -2356,7 +2420,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>114</v>
       </c>
@@ -2373,7 +2437,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>114</v>
       </c>
@@ -2390,7 +2454,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>114</v>
       </c>
@@ -2407,7 +2471,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>114</v>
       </c>
@@ -2424,7 +2488,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>129</v>
       </c>
@@ -2441,7 +2505,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>129</v>
       </c>
@@ -2458,7 +2522,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>129</v>
       </c>
@@ -2475,7 +2539,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>129</v>
       </c>
@@ -2492,7 +2556,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>129</v>
       </c>
@@ -2511,7 +2575,7 @@
       <c r="H73"/>
       <c r="I73"/>
     </row>
-    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>117</v>
       </c>
@@ -2530,7 +2594,7 @@
       <c r="H74"/>
       <c r="I74"/>
     </row>
-    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>117</v>
       </c>
@@ -2549,7 +2613,7 @@
       <c r="H75"/>
       <c r="I75"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>117</v>
       </c>
@@ -2568,7 +2632,7 @@
       <c r="H76"/>
       <c r="I76"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>117</v>
       </c>
@@ -2587,7 +2651,7 @@
       <c r="H77"/>
       <c r="I77"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>117</v>
       </c>
@@ -2606,7 +2670,7 @@
       <c r="H78"/>
       <c r="I78"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>117</v>
       </c>
@@ -2625,7 +2689,7 @@
       <c r="H79"/>
       <c r="I79"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>126</v>
       </c>
@@ -2644,7 +2708,7 @@
       <c r="H80"/>
       <c r="I80"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>126</v>
       </c>
@@ -2663,7 +2727,7 @@
       <c r="H81"/>
       <c r="I81"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>117</v>
       </c>
@@ -2682,7 +2746,7 @@
       <c r="H82"/>
       <c r="I82"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>129</v>
       </c>
@@ -2701,7 +2765,7 @@
       <c r="H83"/>
       <c r="I83"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>126</v>
       </c>
@@ -2717,10 +2781,12 @@
       <c r="G84" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H84"/>
+      <c r="H84" s="9" t="s">
+        <v>225</v>
+      </c>
       <c r="I84"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>126</v>
       </c>
@@ -2736,10 +2802,12 @@
       <c r="G85" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H85"/>
+      <c r="H85" s="9" t="s">
+        <v>226</v>
+      </c>
       <c r="I85"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>126</v>
       </c>
@@ -2755,10 +2823,12 @@
       <c r="G86" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H86"/>
+      <c r="H86" s="10" t="s">
+        <v>227</v>
+      </c>
       <c r="I86"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>126</v>
       </c>
@@ -2774,10 +2844,12 @@
       <c r="G87" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H87"/>
+      <c r="H87" s="10" t="s">
+        <v>228</v>
+      </c>
       <c r="I87"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>122</v>
       </c>
@@ -2793,10 +2865,12 @@
       <c r="G88" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H88"/>
+      <c r="H88" s="10" t="s">
+        <v>227</v>
+      </c>
       <c r="I88"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>122</v>
       </c>
@@ -2812,10 +2886,12 @@
       <c r="G89" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H89"/>
+      <c r="H89" s="10" t="s">
+        <v>229</v>
+      </c>
       <c r="I89"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>126</v>
       </c>
@@ -2831,10 +2907,12 @@
       <c r="G90" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H90"/>
+      <c r="H90" s="10" t="s">
+        <v>227</v>
+      </c>
       <c r="I90"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>126</v>
       </c>
@@ -2850,10 +2928,12 @@
       <c r="G91" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H91"/>
+      <c r="H91" s="10" t="s">
+        <v>230</v>
+      </c>
       <c r="I91"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>126</v>
       </c>
@@ -2869,10 +2949,12 @@
       <c r="G92" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H92"/>
+      <c r="H92" s="9" t="s">
+        <v>231</v>
+      </c>
       <c r="I92"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>126</v>
       </c>
@@ -2888,10 +2970,12 @@
       <c r="G93" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H93"/>
+      <c r="H93" s="10" t="s">
+        <v>227</v>
+      </c>
       <c r="I93"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>126</v>
       </c>
@@ -2907,10 +2991,12 @@
       <c r="G94" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H94"/>
+      <c r="H94" s="10" t="s">
+        <v>232</v>
+      </c>
       <c r="I94"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>126</v>
       </c>
@@ -2926,10 +3012,12 @@
       <c r="G95" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H95"/>
+      <c r="H95" s="10" t="s">
+        <v>233</v>
+      </c>
       <c r="I95"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>126</v>
       </c>
@@ -2945,10 +3033,12 @@
       <c r="G96" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H96"/>
+      <c r="H96" s="10" t="s">
+        <v>234</v>
+      </c>
       <c r="I96"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>126</v>
       </c>
@@ -2964,10 +3054,12 @@
       <c r="G97" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H97"/>
+      <c r="H97" s="10" t="s">
+        <v>227</v>
+      </c>
       <c r="I97"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>126</v>
       </c>
@@ -2983,10 +3075,12 @@
       <c r="G98" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H98"/>
+      <c r="H98" s="11" t="s">
+        <v>235</v>
+      </c>
       <c r="I98"/>
     </row>
-    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>129</v>
       </c>
@@ -3005,7 +3099,7 @@
       <c r="H99"/>
       <c r="I99"/>
     </row>
-    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>129</v>
       </c>
@@ -3024,7 +3118,7 @@
       <c r="H100"/>
       <c r="I100"/>
     </row>
-    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>129</v>
       </c>
@@ -3043,7 +3137,7 @@
       <c r="H101"/>
       <c r="I101"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>129</v>
       </c>
@@ -3062,7 +3156,7 @@
       <c r="H102"/>
       <c r="I102"/>
     </row>
-    <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>117</v>
       </c>
@@ -3086,7 +3180,7 @@
       </c>
       <c r="I103"/>
     </row>
-    <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>117</v>
       </c>
@@ -3110,7 +3204,7 @@
       </c>
       <c r="I104"/>
     </row>
-    <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>117</v>
       </c>
@@ -3134,7 +3228,7 @@
       </c>
       <c r="I105"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>117</v>
       </c>
@@ -3153,7 +3247,7 @@
       <c r="H106"/>
       <c r="I106"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>122</v>
       </c>
@@ -3169,10 +3263,12 @@
       <c r="G107" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H107"/>
+      <c r="H107" s="9" t="s">
+        <v>236</v>
+      </c>
       <c r="I107"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>114</v>
       </c>
@@ -3191,7 +3287,7 @@
       <c r="H108"/>
       <c r="I108"/>
     </row>
-    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>117</v>
       </c>
@@ -3209,6 +3305,22 @@
       </c>
       <c r="H109"/>
       <c r="I109"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B110" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="H110" s="10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B111" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H111" s="10" t="s">
+        <v>240</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>